<commit_message>
note Acquis oke passage au front
</commit_message>
<xml_diff>
--- a/doc/journalTravail.xlsx
+++ b/doc/journalTravail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\P-WebSecutity\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF7AE09-0BAC-4743-8F55-30D646478800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7D4C1A-4486-44CF-BB0E-020D7A75FF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -129,21 +129,6 @@
     <t>P_APP_183 : Secured WebShop</t>
   </si>
   <si>
-    <t>Discussion du projet avec le prof</t>
-  </si>
-  <si>
-    <t>Création repo git + installation VSCode + création dossier dans le repo</t>
-  </si>
-  <si>
-    <t>mise en place du docker</t>
-  </si>
-  <si>
-    <t>Lancement du docker compose + verrification du bon fonctionnement du docker problème: serveur non fonctionnel quand les fichiers sont renommer 30 min d'essaie, problème réglé. Solution: modifier les chaines de caractère comprenons "server.js" dans le fichier "package.json" ainsi que le dockerfile par "app.mjs"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création des maquette: Création de la page de login + palette de couleur </t>
-  </si>
-  <si>
     <t>Absence</t>
   </si>
   <si>
@@ -153,34 +138,58 @@
     <t>Aide mathis + mateen pour exercice Audit</t>
   </si>
   <si>
-    <t>Mise en place du hashage des mot de passe des utilisateur lors de la création</t>
+    <t>Mise en place du certificat + server HTTPS : réuissi</t>
   </si>
   <si>
-    <t>Mise en place de l'authentification avec mdp hashé + mise en place de message d'erreur en cas d'une erreur dans l'authentification</t>
+    <t>mise en place des permission admin dans le payload du token + mise en place de la longueur du sel aléatoire. : réuissi</t>
   </si>
   <si>
-    <t>tentaive automatisation db</t>
+    <t>récupération du sel lors de l'authentification de l'utilisateur afin de comparé le mot de passe : réuissi</t>
   </si>
   <si>
-    <t xml:space="preserve">Récupération de la clef privée depuis un fichier </t>
+    <t>Création de la colonne admin pour les utilisateur + recherche sur le type tinyInt(1) : réuissi</t>
   </si>
   <si>
-    <t xml:space="preserve">Tentative de création d'un token avec la clef privée </t>
+    <t>Ajout du sel lors de la création de l'utilisateur : réuissi</t>
   </si>
   <si>
-    <t>mise en place du token avec la clef privée</t>
+    <t>mise en place du token avec la clef privée : réuissi</t>
   </si>
   <si>
-    <t>Création de la colonne admin pour les utilisateur + recherche sur le type tinyInt(1)</t>
+    <t>Tentative de création d'un token avec la clef privée  : réuissi</t>
   </si>
   <si>
-    <t>Ajout du sel lors de la création de l'utilisateur</t>
+    <t>Récupération de la clef privée depuis un fichier  : réuissi</t>
   </si>
   <si>
-    <t>récupération du sel lors de l'authentification de l'utilisateur afin de comparé le mot de passe</t>
+    <t>tentaive automatisation db : réuissi</t>
   </si>
   <si>
-    <t>mise en place des permission admin dans le payload du token + mise en place de la longueur du sel aléatoire.</t>
+    <t>Mise en place de l'authentification avec mdp hashé + mise en place de message d'erreur en cas d'une erreur dans l'authentification : réuissi</t>
+  </si>
+  <si>
+    <t>Mise en place du hashage des mot de passe des utilisateur lors de la création : réuissi</t>
+  </si>
+  <si>
+    <t>Création des maquette: Création de la page de login + palette de couleur  : réuissi</t>
+  </si>
+  <si>
+    <t>Lancement du docker compose + verrification du bon fonctionnement du docker problème: serveur non fonctionnel quand les fichiers sont renommer 30 min d'essaie, problème réglé. Solution: modifier les chaines de caractère comprenons "server.js" dans le fichier "package.json" ainsi que le dockerfile par "app.mjs"  : réuissi</t>
+  </si>
+  <si>
+    <t>mise en place du docker : réuissi</t>
+  </si>
+  <si>
+    <t>Création repo git + installation VSCode + création dossier dans le repo : réuissi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussion du projet avec le prof </t>
+  </si>
+  <si>
+    <t>Aide Evin + toilet</t>
+  </si>
+  <si>
+    <t>Tentatie création app vue dans docker : echec</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1084,7 @@
                   <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.26041666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1093,7 +1102,7 @@
                   <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3888888888888888E-2</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2005,8 +2014,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2068,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 8 heurs 40 minutes</v>
+        <v>0 jours 11 heurs 5 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2074,15 +2083,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>340</v>
+        <v>425</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>520</v>
+        <v>665</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2132,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="48" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="G7" s="16"/>
     </row>
@@ -2148,7 +2157,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G8" s="17"/>
       <c r="M8" t="s">
@@ -2174,7 +2183,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="48" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G9" s="20"/>
       <c r="M9" t="s">
@@ -2199,7 +2208,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="48" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="G10" s="17"/>
       <c r="M10" t="s">
@@ -2225,7 +2234,7 @@
         <v>24</v>
       </c>
       <c r="F11" s="48" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G11" s="20"/>
       <c r="M11" t="s">
@@ -2250,7 +2259,7 @@
         <v>25</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G12" s="17"/>
       <c r="M12" t="s">
@@ -2276,7 +2285,7 @@
         <v>25</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G13" s="20"/>
       <c r="M13" t="s">
@@ -2299,7 +2308,7 @@
         <v>25</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G14" s="17"/>
       <c r="M14" t="s">
@@ -2323,7 +2332,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="48" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G15" s="20"/>
       <c r="M15" t="s">
@@ -2346,7 +2355,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="48" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G16" s="17"/>
       <c r="O16">
@@ -2364,7 +2373,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G17" s="20"/>
       <c r="O17">
@@ -2383,7 +2392,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="17"/>
       <c r="O18">
@@ -2401,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G19" s="20"/>
       <c r="O19">
@@ -2418,7 +2427,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G20" s="17"/>
     </row>
@@ -2433,7 +2442,7 @@
         <v>4</v>
       </c>
       <c r="F21" s="48" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G21" s="20"/>
     </row>
@@ -2447,7 +2456,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="48" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G22" s="17"/>
     </row>
@@ -2462,11 +2471,11 @@
         <v>4</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G23" s="20"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="39"/>
       <c r="C24" s="35"/>
       <c r="D24" s="43">
@@ -2476,11 +2485,11 @@
         <v>4</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="40"/>
       <c r="C25" s="36"/>
@@ -2491,7 +2500,7 @@
         <v>4</v>
       </c>
       <c r="F25" s="48" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G25" s="20"/>
     </row>
@@ -2505,33 +2514,56 @@
         <v>4</v>
       </c>
       <c r="F26" s="48" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="48"/>
+      <c r="B27" s="40">
+        <v>45429</v>
+      </c>
+      <c r="C27" s="36">
+        <v>1</v>
+      </c>
+      <c r="D27" s="44">
+        <v>40</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="39"/>
       <c r="C28" s="35"/>
-      <c r="D28" s="43"/>
-      <c r="F28" s="47"/>
+      <c r="D28" s="43">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>48</v>
+      </c>
       <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="40"/>
       <c r="C29" s="36"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="47"/>
+      <c r="D29" s="44">
+        <v>35</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>49</v>
+      </c>
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8330,11 +8362,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>240</v>
+        <v>315</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8342,7 +8374,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.16666666666666666</v>
+        <v>0.26041666666666669</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8434,7 +8466,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C11" s="51" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8442,7 +8474,7 @@
       </c>
       <c r="D11" s="45">
         <f t="shared" si="0"/>
-        <v>1.3888888888888888E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8451,7 +8483,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.2361111111111111</v>
+        <v>0.33680555555555552</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8730,6 +8762,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8739,15 +8780,6 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8771,6 +8803,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8782,12 +8822,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>